<commit_message>
feat: comparison and results cross_validation
</commit_message>
<xml_diff>
--- a/Results/less_constraints_results.xlsx
+++ b/Results/less_constraints_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcoturetta/Projects/trees/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05509848-71F2-8547-828E-29299EF82971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E610C-41F7-6A42-AC56-9B6839DBC719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15580" xr2:uid="{E372065B-5D18-2940-85FF-2A151252FCB1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="less_constra" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="temp_results" localSheetId="0">less_constra!$A$22:$J$25</definedName>
     <definedName name="temp_results_1" localSheetId="0">less_constra!$A$2:$J$9</definedName>
     <definedName name="temp_results_2" localSheetId="0">less_constra!$A$10:$J$17</definedName>
     <definedName name="temp_results_3" localSheetId="0">less_constra!$A$18:$J$21</definedName>
@@ -43,7 +44,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{C57512E9-C8E8-4949-B49A-4B8B0C8735CF}" name="temp_results" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -59,7 +60,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{BD0AB721-AD35-604D-99EE-02B53125565A}" name="temp_results1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" tab="0" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -75,7 +76,23 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{FB983B41-C05C-D04C-9AF8-2E5EA3FF7C9F}" name="temp_results2" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" tab="0" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{B0B762CF-2D10-7746-86F4-1E1C87733AE5}" name="temp_results3" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/temp_results.csv" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -94,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
   <si>
     <t>model</t>
   </si>
@@ -207,15 +224,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="temp_results" connectionId="4" xr16:uid="{28B0956E-71F7-B44E-A772-558039C93E4B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="temp_results_3" connectionId="3" xr16:uid="{D6AF88DF-5C14-E04A-AE76-5370B670FC97}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="temp_results_1" connectionId="1" xr16:uid="{15C44A8F-2978-C146-862C-E756311723CA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="temp_results_2" connectionId="2" xr16:uid="{10A1B104-BAFA-2049-8DE6-DE2B9932FF0B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="temp_results_3" connectionId="3" xr16:uid="{D6AF88DF-5C14-E04A-AE76-5370B670FC97}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,24 +537,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1848F4B-E40A-B344-951D-D2E7E2949231}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="1" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -1208,6 +1223,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>35.093054962158199</v>
+      </c>
+      <c r="G22">
+        <v>0.220231543760955</v>
+      </c>
+      <c r="H22">
+        <v>0.246868753137409</v>
+      </c>
+      <c r="I22">
+        <v>0.26720779220779201</v>
+      </c>
+      <c r="J22">
+        <v>8.0119047619047604E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>81.709550523757898</v>
+      </c>
+      <c r="G23">
+        <v>0.220231543760955</v>
+      </c>
+      <c r="H23">
+        <v>0.246868753137409</v>
+      </c>
+      <c r="I23">
+        <v>0.26720779220779201</v>
+      </c>
+      <c r="J23">
+        <v>7.8214285714285695E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>18.495517063140799</v>
+      </c>
+      <c r="G24">
+        <v>0.220231543760955</v>
+      </c>
+      <c r="H24">
+        <v>0.246868753137409</v>
+      </c>
+      <c r="I24">
+        <v>0.26720779220779201</v>
+      </c>
+      <c r="J24">
+        <v>8.0119047619047604E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-3.0235861096174401E-15</v>
+      </c>
+      <c r="F25">
+        <v>11.6013823509216</v>
+      </c>
+      <c r="G25">
+        <v>0.220231543760955</v>
+      </c>
+      <c r="H25">
+        <v>0.246868753137409</v>
+      </c>
+      <c r="I25">
+        <v>0.270844155844155</v>
+      </c>
+      <c r="J25">
+        <v>6.7103174603174595E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>